<commit_message>
Umsetzung "Satz > Besonderheit"
</commit_message>
<xml_diff>
--- a/helpers/Spalten.xlsx
+++ b/helpers/Spalten.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13440" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="13440" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -98,14 +99,58 @@
   </si>
   <si>
     <t>Standort</t>
+  </si>
+  <si>
+    <t>Verwendungszweck</t>
+  </si>
+  <si>
+    <t>Besetzung</t>
+  </si>
+  <si>
+    <t>Notenwert</t>
+  </si>
+  <si>
+    <t>Strichart</t>
+  </si>
+  <si>
+    <t>Übung</t>
+  </si>
+  <si>
+    <t>Melodische Besonderheit</t>
+  </si>
+  <si>
+    <t>Dynamische Besonderheit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhythmische Besonderheit </t>
+  </si>
+  <si>
+    <t>Relation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL </t>
+  </si>
+  <si>
+    <t>musikstueck</t>
+  </si>
+  <si>
+    <t>satz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,8 +178,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -441,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2036,4 +2082,180 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"INSERT INTO category (Name, Relation) VALUES('" &amp; A2 &amp; "', '" &amp; B2 &amp; "') ;"</f>
+        <v>INSERT INTO category (Name, Relation) VALUES('Verwendungszweck', 'musikstueck') ;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C13" si="0">"INSERT INTO category (Name, Relation) VALUES('" &amp; A3 &amp; "', '" &amp; B3 &amp; "') ;"</f>
+        <v>INSERT INTO category (Name, Relation) VALUES('Besetzung', 'musikstueck') ;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Epoche', 'musikstueck') ;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Gattung', 'musikstueck') ;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Erprobt', 'satz') ;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Notenwert', 'satz') ;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Schwierigkeitsgrad', 'satz') ;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Strichart', 'satz') ;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Übung', 'satz') ;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Melodische Besonderheit', 'satz') ;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Dynamische Besonderheit', 'satz') ;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO category (Name, Relation) VALUES('Rhythmische Besonderheit ', 'satz') ;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>